<commit_message>
Minor changes to the main.py file and the historicals.xlsx file. The historicals-small.xlsx file is untracked and will not be included in the commit.
</commit_message>
<xml_diff>
--- a/historicals.xlsx
+++ b/historicals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AsherKlug\Documents\witness_calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EDCB6C-A7D9-4F0F-8B49-C96206A4DF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3128BA9-4411-41EB-BAD7-CFF10BECC82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ED2F4219-27BD-4A7B-9484-FE82FFA5C270}"/>
   </bookViews>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3240DC-3887-4511-ABB2-AFC9F5D5C9A7}">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>